<commit_message>
Excel changes: frozed headers, fixed default excel position
</commit_message>
<xml_diff>
--- a/django_api/django_api/apps/cluster/templates/excel/export.xlsx
+++ b/django_api/django_api/apps/cluster/templates/excel/export.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Cluster</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>#adm5+code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -699,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU956"/>
+  <dimension ref="A1:AQ956"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA9" sqref="AA9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -911,7 +914,9 @@
       <c r="AQ2" s="1"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>

</xml_diff>